<commit_message>
9/26 testing new pull/commit request changes
</commit_message>
<xml_diff>
--- a/azOmni.xlsx
+++ b/azOmni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTtest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D32446-D2E9-4685-BE3C-64684E60812D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB33C46-A406-4684-A6BB-1CA56C3AE7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="794" firstSheet="3" activeTab="5" xr2:uid="{6959074F-409A-4A24-8EEB-7A54C4A5F3A4}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="266">
   <si>
     <t>version</t>
   </si>
@@ -3141,6 +3141,9 @@
   </si>
   <si>
     <t>this is a test for today 09-26</t>
+  </si>
+  <si>
+    <t>testing new pull request constraints</t>
   </si>
 </sst>
 </file>
@@ -14094,10 +14097,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C418DF-F21F-4428-9E04-0423603B6D5E}">
-  <dimension ref="E1:O8"/>
+  <dimension ref="E1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14146,6 +14149,11 @@
     <row r="8" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
         <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
9/26 testing new pull/commit request changes with !
</commit_message>
<xml_diff>
--- a/azOmni.xlsx
+++ b/azOmni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTtest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB33C46-A406-4684-A6BB-1CA56C3AE7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58548EEE-55A6-4C5B-B28E-8DE1FC634C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="794" firstSheet="3" activeTab="5" xr2:uid="{6959074F-409A-4A24-8EEB-7A54C4A5F3A4}"/>
   </bookViews>
@@ -3143,7 +3143,7 @@
     <t>this is a test for today 09-26</t>
   </si>
   <si>
-    <t>testing new pull request constraints</t>
+    <t>testing new pull request constraints!</t>
   </si>
 </sst>
 </file>
@@ -14100,7 +14100,7 @@
   <dimension ref="E1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
9/30 testing new pull/commit request changes with !
</commit_message>
<xml_diff>
--- a/azOmni.xlsx
+++ b/azOmni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTtest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58548EEE-55A6-4C5B-B28E-8DE1FC634C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309E0AE8-5BDA-4E42-A01F-0300D92F0722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="794" firstSheet="3" activeTab="5" xr2:uid="{6959074F-409A-4A24-8EEB-7A54C4A5F3A4}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="267">
   <si>
     <t>version</t>
   </si>
@@ -3144,6 +3144,9 @@
   </si>
   <si>
     <t>testing new pull request constraints!</t>
+  </si>
+  <si>
+    <t>Testing 9-30</t>
   </si>
 </sst>
 </file>
@@ -14097,10 +14100,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C418DF-F21F-4428-9E04-0423603B6D5E}">
-  <dimension ref="E1:O9"/>
+  <dimension ref="E1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14154,6 +14157,11 @@
     <row r="9" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E9" t="s">
         <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
10/1 testing new pull/commit request changes with !
</commit_message>
<xml_diff>
--- a/azOmni.xlsx
+++ b/azOmni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTtest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309E0AE8-5BDA-4E42-A01F-0300D92F0722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA0367F-6A79-4C7C-BEFB-5478AB6F999A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="794" firstSheet="3" activeTab="5" xr2:uid="{6959074F-409A-4A24-8EEB-7A54C4A5F3A4}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="268">
   <si>
     <t>version</t>
   </si>
@@ -3147,6 +3147,9 @@
   </si>
   <si>
     <t>Testing 9-30</t>
+  </si>
+  <si>
+    <t>Testing 10-1</t>
   </si>
 </sst>
 </file>
@@ -14100,10 +14103,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C418DF-F21F-4428-9E04-0423603B6D5E}">
-  <dimension ref="E1:O10"/>
+  <dimension ref="E1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14162,6 +14165,11 @@
     <row r="10" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
         <v>266</v>
+      </c>
+    </row>
+    <row r="11" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>